<commit_message>
PROS-8723 - MARSRU - fixes for new pandas version compatibility
</commit_message>
<xml_diff>
--- a/Projects/MARSRU2_SAND/Data/2019/MARS KPIs.xlsx
+++ b/Projects/MARSRU2_SAND/Data/2019/MARS KPIs.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="992" firstSheet="0" activeTab="5"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="KPIs_Grocery" sheetId="1" state="visible" r:id="rId2"/>
@@ -23,7 +23,7 @@
   </sheets>
   <definedNames>
     <definedName function="false" hidden="true" localSheetId="5" name="_xlnm._FilterDatabase" vbProcedure="false">'4254'!$A$1:$J$259</definedName>
-    <definedName function="false" hidden="true" localSheetId="1" name="_xlnm._FilterDatabase" vbProcedure="false">KPIs_Drogerie!$A$1:$AA$3</definedName>
+    <definedName function="false" hidden="true" localSheetId="1" name="_xlnm._FilterDatabase" vbProcedure="false">KPIs_Drogerie!$A$1:$AA$27</definedName>
     <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">KPIs_Grocery!$A$1:$AA$56</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">KPIs_Grocery!$A$1:$AA$56</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0" vbProcedure="false">KPIs_Grocery!$A$1:$AA$56</definedName>
@@ -34,6 +34,7 @@
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0" vbProcedure="false">KPIs_Grocery!$A$1:$AA$56</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0" vbProcedure="false">KPIs_Grocery!$A$1:$AA$56</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0" vbProcedure="false">KPIs_Grocery!$A$1:$AA$56</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0" vbProcedure="false">KPIs_Grocery!$A$1:$AA$56</definedName>
     <definedName function="false" hidden="false" localSheetId="1" name="_FilterDatabase_0" vbProcedure="false">KPIs_Drogerie!$B$1:$AA$1</definedName>
     <definedName function="false" hidden="false" localSheetId="1" name="_FilterDatabase_0_0" vbProcedure="false">KPIs_Drogerie!$B$1:$AA$1</definedName>
     <definedName function="false" hidden="false" localSheetId="1" name="_FilterDatabase_0_0_0" vbProcedure="false">KPIs_Drogerie!$B$1:$AA$1</definedName>
@@ -48,16 +49,16 @@
     <definedName function="false" hidden="false" localSheetId="1" name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">KPIs_Drogerie!$B$1:$AA$1</definedName>
     <definedName function="false" hidden="false" localSheetId="1" name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">KPIs_Drogerie!$B$1:$AA$1</definedName>
     <definedName function="false" hidden="false" localSheetId="1" name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">KPIs_Drogerie!$B$1:$AA$1</definedName>
-    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase" vbProcedure="false">KPIs_Drogerie!$A$1:$AA$27</definedName>
-    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0" vbProcedure="false">KPIs_Drogerie!$A$1:$AA$3</definedName>
-    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">KPIs_Drogerie!$A$1:$AA$27</definedName>
-    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0_0" vbProcedure="false">KPIs_Drogerie!$A$1:$AA$3</definedName>
-    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0_0_0" vbProcedure="false">KPIs_Drogerie!$A$1:$AA$27</definedName>
-    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0_0_0_0" vbProcedure="false">KPIs_Drogerie!$A$1:$AA$3</definedName>
-    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0_0_0_0_0" vbProcedure="false">KPIs_Drogerie!$A$1:$AA$27</definedName>
-    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0" vbProcedure="false">KPIs_Drogerie!$A$1:$AA$3</definedName>
-    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0" vbProcedure="false">KPIs_Drogerie!$A$1:$AA$27</definedName>
-    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0" vbProcedure="false">KPIs_Drogerie!$A$1:$AA$3</definedName>
+    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase" vbProcedure="false">KPIs_Drogerie!$A$1:$AA$3</definedName>
+    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0" vbProcedure="false">KPIs_Drogerie!$A$1:$AA$27</definedName>
+    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">KPIs_Drogerie!$A$1:$AA$3</definedName>
+    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0_0" vbProcedure="false">KPIs_Drogerie!$A$1:$AA$27</definedName>
+    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0_0_0" vbProcedure="false">KPIs_Drogerie!$A$1:$AA$3</definedName>
+    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0_0_0_0" vbProcedure="false">KPIs_Drogerie!$A$1:$AA$27</definedName>
+    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0_0_0_0_0" vbProcedure="false">KPIs_Drogerie!$A$1:$AA$3</definedName>
+    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0" vbProcedure="false">KPIs_Drogerie!$A$1:$AA$27</definedName>
+    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0" vbProcedure="false">KPIs_Drogerie!$A$1:$AA$3</definedName>
+    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0" vbProcedure="false">KPIs_Drogerie!$A$1:$AA$27</definedName>
     <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">KPIs_Drogerie!$A$1:$AA$3</definedName>
     <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">KPIs_Drogerie!$A$1:$AA$3</definedName>
     <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">KPIs_Drogerie!$A$1:$AA$3</definedName>
@@ -82,6 +83,7 @@
     <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">KPIs_Drogerie!$A$1:$AA$3</definedName>
     <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">KPIs_Drogerie!$A$1:$AA$3</definedName>
     <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">KPIs_Drogerie!$A$1:$AA$3</definedName>
+    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">KPIs_Drogerie!$A$1:$AA$3</definedName>
     <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase" vbProcedure="false">'4317'!$A$1:$C$54</definedName>
     <definedName function="false" hidden="false" localSheetId="5" name="_xlnm._FilterDatabase" vbProcedure="false">'4254'!$A$1:$J$259</definedName>
     <definedName function="false" hidden="false" localSheetId="5" name="_xlnm._FilterDatabase_0" vbProcedure="false">'4254'!$A$1:$J$259</definedName>
@@ -104,10 +106,11 @@
     <definedName function="false" hidden="false" localSheetId="5" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'4254'!$A$1:$J$259</definedName>
     <definedName function="false" hidden="false" localSheetId="5" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'4254'!$A$1:$J$259</definedName>
     <definedName function="false" hidden="false" localSheetId="5" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'4254'!$A$1:$J$259</definedName>
-    <definedName function="false" hidden="false" localSheetId="5" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'4254'!$A$2:$J$260</definedName>
-    <definedName function="false" hidden="false" localSheetId="5" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'4254'!$A$1:$J$259</definedName>
-    <definedName function="false" hidden="false" localSheetId="5" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'4254'!$A$2:$J$260</definedName>
+    <definedName function="false" hidden="false" localSheetId="5" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'4254'!$A$1:$J$259</definedName>
+    <definedName function="false" hidden="false" localSheetId="5" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'4254'!$A$2:$J$260</definedName>
+    <definedName function="false" hidden="false" localSheetId="5" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'4254'!$A$1:$J$259</definedName>
     <definedName function="false" hidden="false" localSheetId="5" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'4254'!$A$2:$J$260</definedName>
+    <definedName function="false" hidden="false" localSheetId="5" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'4254'!$A$2:$J$260</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -119,7 +122,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3048" uniqueCount="346">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3053" uniqueCount="346">
   <si>
     <t xml:space="preserve">Comment</t>
   </si>
@@ -430,6 +433,9 @@
   </si>
   <si>
     <t xml:space="preserve">MAN in CAT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mars</t>
   </si>
   <si>
     <t xml:space="preserve">Суммарный размер выкладки всей категории (в метрах)на всех полках для категорий кошки (включая лакомства на основной полке, БЕЗ НАПОЛНИТЕЛЕЙ)</t>
@@ -714,9 +720,6 @@
   </si>
   <si>
     <t xml:space="preserve">Hanger MARS Cat</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mars</t>
   </si>
   <si>
     <t xml:space="preserve">Количество навесок с лакомтсвами собак (dentastix)</t>
@@ -1714,28 +1717,28 @@
   </sheetPr>
   <dimension ref="A1:AA56"/>
   <sheetViews>
-    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="I42" activePane="bottomRight" state="frozen"/>
+    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="3" ySplit="1" topLeftCell="D38" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="I1" activeCellId="0" sqref="I1"/>
-      <selection pane="bottomLeft" activeCell="A42" activeCellId="0" sqref="A42"/>
-      <selection pane="bottomRight" activeCell="I38" activeCellId="1" sqref="B57:B60 I38"/>
+      <selection pane="topRight" activeCell="D1" activeCellId="0" sqref="D1"/>
+      <selection pane="bottomLeft" activeCell="A38" activeCellId="0" sqref="A38"/>
+      <selection pane="bottomRight" activeCell="A42" activeCellId="0" sqref="A42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="1" width="13.3886639676113"/>
     <col collapsed="false" hidden="false" max="5" min="2" style="2" width="13.3886639676113"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="2" width="29.5668016194332"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="2" width="101.761133603239"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="2" width="71.4493927125506"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="2" width="30.2064777327935"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="2" width="29.7773279352227"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="2" width="102.728744939271"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="2" width="72.0890688259109"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="2" width="30.4210526315789"/>
     <col collapsed="false" hidden="false" max="10" min="10" style="2" width="16.3886639676113"/>
     <col collapsed="false" hidden="false" max="14" min="11" style="2" width="13.3886639676113"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="3" width="36.8502024291498"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="3" width="37.17004048583"/>
     <col collapsed="false" hidden="false" max="16" min="16" style="3" width="13.497975708502"/>
     <col collapsed="false" hidden="false" max="17" min="17" style="2" width="13.497975708502"/>
-    <col collapsed="false" hidden="false" max="18" min="18" style="2" width="20.995951417004"/>
+    <col collapsed="false" hidden="false" max="18" min="18" style="2" width="21.1012145748988"/>
     <col collapsed="false" hidden="false" max="27" min="19" style="2" width="13.497975708502"/>
     <col collapsed="false" hidden="false" max="1025" min="28" style="1" width="9.10526315789474"/>
   </cols>
@@ -3068,7 +3071,9 @@
       <c r="O23" s="10" t="s">
         <v>35</v>
       </c>
-      <c r="P23" s="10"/>
+      <c r="P23" s="10" t="s">
+        <v>93</v>
+      </c>
       <c r="Q23" s="10" t="s">
         <v>36</v>
       </c>
@@ -3101,10 +3106,10 @@
         <v>28</v>
       </c>
       <c r="G24" s="10" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="H24" s="10" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="I24" s="10" t="s">
         <v>91</v>
@@ -3158,16 +3163,16 @@
         <v>28</v>
       </c>
       <c r="G25" s="10" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="H25" s="10" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="I25" s="10" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="J25" s="10" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="K25" s="10" t="s">
         <v>80</v>
@@ -3180,7 +3185,7 @@
       </c>
       <c r="N25" s="10"/>
       <c r="O25" s="10" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="P25" s="10"/>
       <c r="Q25" s="10"/>
@@ -3215,10 +3220,10 @@
         <v>28</v>
       </c>
       <c r="G26" s="10" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="H26" s="10" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="I26" s="10" t="s">
         <v>91</v>
@@ -3230,7 +3235,7 @@
         <v>33</v>
       </c>
       <c r="L26" s="10" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="M26" s="10" t="n">
         <v>0</v>
@@ -3239,7 +3244,9 @@
       <c r="O26" s="10" t="s">
         <v>39</v>
       </c>
-      <c r="P26" s="10"/>
+      <c r="P26" s="10" t="s">
+        <v>93</v>
+      </c>
       <c r="Q26" s="10" t="s">
         <v>36</v>
       </c>
@@ -3272,10 +3279,10 @@
         <v>28</v>
       </c>
       <c r="G27" s="10" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="H27" s="10" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="I27" s="10" t="s">
         <v>91</v>
@@ -3326,19 +3333,19 @@
         <v>27</v>
       </c>
       <c r="F28" s="10" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="G28" s="10" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="H28" s="13" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="I28" s="10" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="J28" s="10" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="K28" s="10" t="s">
         <v>80</v>
@@ -3379,19 +3386,19 @@
         <v>27</v>
       </c>
       <c r="F29" s="10" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="G29" s="10" t="s">
+        <v>111</v>
+      </c>
+      <c r="H29" s="13" t="s">
+        <v>112</v>
+      </c>
+      <c r="I29" s="10" t="s">
+        <v>109</v>
+      </c>
+      <c r="J29" s="10" t="s">
         <v>110</v>
-      </c>
-      <c r="H29" s="13" t="s">
-        <v>111</v>
-      </c>
-      <c r="I29" s="10" t="s">
-        <v>108</v>
-      </c>
-      <c r="J29" s="10" t="s">
-        <v>109</v>
       </c>
       <c r="K29" s="10" t="s">
         <v>80</v>
@@ -3432,19 +3439,19 @@
         <v>27</v>
       </c>
       <c r="F30" s="10" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="G30" s="10" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="H30" s="13" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="I30" s="10" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="J30" s="10" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="K30" s="10" t="s">
         <v>80</v>
@@ -3485,19 +3492,19 @@
         <v>27</v>
       </c>
       <c r="F31" s="10" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="G31" s="10" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="H31" s="13" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="I31" s="10" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="J31" s="10" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="K31" s="10" t="s">
         <v>80</v>
@@ -3541,16 +3548,16 @@
         <v>28</v>
       </c>
       <c r="G32" s="10" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="H32" s="10" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="I32" s="10" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="J32" s="10" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="K32" s="10" t="s">
         <v>80</v>
@@ -3563,7 +3570,7 @@
       </c>
       <c r="N32" s="10"/>
       <c r="O32" s="10" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="P32" s="10"/>
       <c r="Q32" s="10"/>
@@ -3598,16 +3605,16 @@
         <v>76</v>
       </c>
       <c r="G33" s="10" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="H33" s="13" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="I33" s="10" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="J33" s="10" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="K33" s="10" t="s">
         <v>80</v>
@@ -3620,7 +3627,7 @@
       </c>
       <c r="N33" s="10"/>
       <c r="O33" s="10" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="P33" s="10"/>
       <c r="Q33" s="10" t="s">
@@ -3628,14 +3635,14 @@
       </c>
       <c r="R33" s="10"/>
       <c r="S33" s="10" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="T33" s="10"/>
       <c r="U33" s="10"/>
       <c r="V33" s="10"/>
       <c r="W33" s="10"/>
       <c r="X33" s="10" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="Y33" s="10"/>
       <c r="Z33" s="10"/>
@@ -3659,16 +3666,16 @@
         <v>76</v>
       </c>
       <c r="G34" s="10" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="H34" s="10" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="I34" s="10" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="J34" s="10" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="K34" s="10" t="s">
         <v>80</v>
@@ -3681,7 +3688,9 @@
       <c r="O34" s="10" t="n">
         <v>4306</v>
       </c>
-      <c r="P34" s="10"/>
+      <c r="P34" s="10" t="s">
+        <v>93</v>
+      </c>
       <c r="Q34" s="10"/>
       <c r="R34" s="10"/>
       <c r="S34" s="10"/>
@@ -3709,19 +3718,19 @@
         <v>27</v>
       </c>
       <c r="F35" s="10" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="G35" s="10" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="H35" s="13" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="I35" s="10" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="J35" s="10" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="K35" s="10" t="s">
         <v>80</v>
@@ -3762,19 +3771,19 @@
         <v>27</v>
       </c>
       <c r="F36" s="10" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="G36" s="10" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="H36" s="13" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="I36" s="10" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="J36" s="10" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="K36" s="10" t="s">
         <v>80</v>
@@ -3815,19 +3824,19 @@
         <v>27</v>
       </c>
       <c r="F37" s="10" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="G37" s="10" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="H37" s="13" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="I37" s="10" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="J37" s="10" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="K37" s="10" t="s">
         <v>80</v>
@@ -3868,19 +3877,19 @@
         <v>27</v>
       </c>
       <c r="F38" s="10" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="G38" s="10" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="H38" s="13" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="I38" s="10" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="J38" s="10" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="K38" s="10" t="s">
         <v>80</v>
@@ -3924,16 +3933,16 @@
         <v>76</v>
       </c>
       <c r="G39" s="10" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="H39" s="10" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="I39" s="10" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="J39" s="10" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="K39" s="10" t="s">
         <v>80</v>
@@ -3977,16 +3986,16 @@
         <v>76</v>
       </c>
       <c r="G40" s="10" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="H40" s="10" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="I40" s="10" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="J40" s="10" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="K40" s="10" t="s">
         <v>80</v>
@@ -4030,16 +4039,16 @@
         <v>76</v>
       </c>
       <c r="G41" s="10" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="H41" s="10" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="I41" s="10" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="J41" s="10" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="K41" s="10" t="s">
         <v>80</v>
@@ -4083,10 +4092,10 @@
         <v>76</v>
       </c>
       <c r="G42" s="10" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="H42" s="14" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="I42" s="10" t="s">
         <v>79</v>
@@ -4101,7 +4110,7 @@
       <c r="M42" s="10"/>
       <c r="N42" s="10"/>
       <c r="O42" s="15" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="P42" s="15"/>
       <c r="Q42" s="10" t="s">
@@ -4136,10 +4145,10 @@
         <v>76</v>
       </c>
       <c r="G43" s="10" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="H43" s="12" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="I43" s="10" t="s">
         <v>79</v>
@@ -4154,7 +4163,7 @@
       <c r="M43" s="10"/>
       <c r="N43" s="10"/>
       <c r="O43" s="13" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="P43" s="10"/>
       <c r="Q43" s="10" t="s">
@@ -4189,13 +4198,13 @@
         <v>76</v>
       </c>
       <c r="G44" s="10" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="H44" s="14" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="I44" s="10" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="J44" s="10"/>
       <c r="K44" s="10" t="s">
@@ -4207,7 +4216,7 @@
       <c r="M44" s="10"/>
       <c r="N44" s="10"/>
       <c r="O44" s="13" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="P44" s="10"/>
       <c r="Q44" s="10" t="s">
@@ -4222,7 +4231,7 @@
       <c r="V44" s="10"/>
       <c r="W44" s="10"/>
       <c r="X44" s="10" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="Y44" s="10"/>
       <c r="Z44" s="10"/>
@@ -4243,16 +4252,16 @@
         <v>27</v>
       </c>
       <c r="F45" s="10" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="G45" s="10" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="H45" s="12" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="I45" s="10" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="J45" s="10"/>
       <c r="K45" s="10" t="s">
@@ -4264,7 +4273,7 @@
       <c r="M45" s="10"/>
       <c r="N45" s="10"/>
       <c r="O45" s="13" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="P45" s="10"/>
       <c r="Q45" s="10" t="s">
@@ -4296,16 +4305,16 @@
         <v>27</v>
       </c>
       <c r="F46" s="10" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="G46" s="10" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="H46" s="12" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="I46" s="10" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="J46" s="10"/>
       <c r="K46" s="10" t="s">
@@ -4349,16 +4358,16 @@
         <v>27</v>
       </c>
       <c r="F47" s="10" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="G47" s="10" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="H47" s="12" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="I47" s="10" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="J47" s="10"/>
       <c r="K47" s="10" t="s">
@@ -4370,11 +4379,11 @@
       <c r="M47" s="10"/>
       <c r="N47" s="10"/>
       <c r="O47" s="10" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="P47" s="10"/>
       <c r="Q47" s="10" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="R47" s="10"/>
       <c r="S47" s="10"/>
@@ -4402,19 +4411,19 @@
         <v>27</v>
       </c>
       <c r="F48" s="10" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="G48" s="10" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="H48" s="10" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="I48" s="10" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="J48" s="10" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="K48" s="10" t="s">
         <v>42</v>
@@ -4425,12 +4434,12 @@
       <c r="M48" s="10"/>
       <c r="N48" s="10"/>
       <c r="O48" s="10" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="P48" s="10"/>
       <c r="Q48" s="10"/>
       <c r="R48" s="10" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="S48" s="10"/>
       <c r="T48" s="10"/>
@@ -4455,19 +4464,19 @@
         <v>27</v>
       </c>
       <c r="F49" s="10" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="G49" s="10" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="H49" s="10" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="I49" s="10" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="J49" s="10" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="K49" s="10" t="s">
         <v>42</v>
@@ -4478,14 +4487,14 @@
       <c r="M49" s="10"/>
       <c r="N49" s="10"/>
       <c r="O49" s="10" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="P49" s="10" t="s">
-        <v>167</v>
+        <v>93</v>
       </c>
       <c r="Q49" s="10"/>
       <c r="R49" s="10" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="S49" s="10" t="s">
         <v>35</v>
@@ -4512,7 +4521,7 @@
         <v>27</v>
       </c>
       <c r="F50" s="10" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="G50" s="10" t="s">
         <v>168</v>
@@ -4521,10 +4530,10 @@
         <v>169</v>
       </c>
       <c r="I50" s="10" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="J50" s="10" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="K50" s="10" t="s">
         <v>42</v>
@@ -4538,7 +4547,7 @@
         <v>170</v>
       </c>
       <c r="P50" s="10" t="s">
-        <v>167</v>
+        <v>93</v>
       </c>
       <c r="Q50" s="10"/>
       <c r="R50" s="10" t="s">
@@ -4569,7 +4578,7 @@
         <v>27</v>
       </c>
       <c r="F51" s="10" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="G51" s="10" t="s">
         <v>171</v>
@@ -4581,7 +4590,7 @@
         <v>173</v>
       </c>
       <c r="J51" s="10" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="K51" s="10" t="s">
         <v>80</v>
@@ -4597,7 +4606,7 @@
         <v>174</v>
       </c>
       <c r="P51" s="10" t="s">
-        <v>167</v>
+        <v>93</v>
       </c>
       <c r="Q51" s="10"/>
       <c r="R51" s="10" t="s">
@@ -4626,7 +4635,7 @@
         <v>27</v>
       </c>
       <c r="F52" s="10" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="G52" s="10" t="s">
         <v>175</v>
@@ -4638,7 +4647,7 @@
         <v>173</v>
       </c>
       <c r="J52" s="10" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="K52" s="10" t="s">
         <v>80</v>
@@ -4654,7 +4663,7 @@
         <v>177</v>
       </c>
       <c r="P52" s="10" t="s">
-        <v>167</v>
+        <v>93</v>
       </c>
       <c r="Q52" s="10"/>
       <c r="R52" s="10" t="s">
@@ -4683,19 +4692,19 @@
         <v>27</v>
       </c>
       <c r="F53" s="10" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="G53" s="10" t="s">
         <v>178</v>
       </c>
       <c r="H53" s="13" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="I53" s="10" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="J53" s="10" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="K53" s="10" t="s">
         <v>80</v>
@@ -4734,19 +4743,19 @@
         <v>27</v>
       </c>
       <c r="F54" s="10" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="G54" s="10" t="s">
         <v>179</v>
       </c>
       <c r="H54" s="13" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="I54" s="10" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="J54" s="10" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="K54" s="10" t="s">
         <v>80</v>
@@ -4785,19 +4794,19 @@
         <v>27</v>
       </c>
       <c r="F55" s="10" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="G55" s="10" t="s">
         <v>180</v>
       </c>
       <c r="H55" s="13" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="I55" s="10" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="J55" s="10" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="K55" s="10" t="s">
         <v>80</v>
@@ -4836,19 +4845,19 @@
         <v>27</v>
       </c>
       <c r="F56" s="10" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="G56" s="10" t="s">
         <v>181</v>
       </c>
       <c r="H56" s="13" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="I56" s="10" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="J56" s="10" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="K56" s="10" t="s">
         <v>80</v>
@@ -4895,14 +4904,14 @@
   <dimension ref="A1:C1"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="B57:B60 A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="19" width="13.3886639676113"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="41.5627530364373"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="19" width="20.6720647773279"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="41.8825910931174"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="19" width="20.7813765182186"/>
     <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
@@ -4936,15 +4945,15 @@
   <dimension ref="A1:B14"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B22" activeCellId="1" sqref="B57:B60 B22"/>
+      <selection pane="topLeft" activeCell="B22" activeCellId="0" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="38.2429149797571"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="37.5991902834008"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="38.5627530364372"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="37.8137651821862"/>
     <col collapsed="false" hidden="false" max="5" min="3" style="0" width="8.57085020242915"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="35.8866396761134"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="36.2064777327935"/>
     <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
@@ -5079,12 +5088,12 @@
   <dimension ref="A1:A65536"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A18" activeCellId="1" sqref="B57:B60 A18"/>
+      <selection pane="topLeft" activeCell="A18" activeCellId="0" sqref="A18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="51.5222672064777"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="51.9514170040486"/>
     <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
@@ -5149,27 +5158,27 @@
   <dimension ref="A1:AA28"/>
   <sheetViews>
     <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="1" topLeftCell="D10" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="D1" activeCellId="0" sqref="D1"/>
-      <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A12" activeCellId="1" sqref="B57:B60 A12"/>
+      <selection pane="bottomLeft" activeCell="A10" activeCellId="0" sqref="A10"/>
+      <selection pane="bottomRight" activeCell="A25" activeCellId="0" sqref="A25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="1" width="13.3886639676113"/>
     <col collapsed="false" hidden="false" max="5" min="2" style="2" width="13.3886639676113"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="2" width="29.5668016194332"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="2" width="101.761133603239"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="2" width="71.4493927125506"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="2" width="30.2064777327935"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="2" width="29.7773279352227"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="2" width="102.728744939271"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="2" width="72.0890688259109"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="2" width="30.4210526315789"/>
     <col collapsed="false" hidden="false" max="10" min="10" style="2" width="16.3886639676113"/>
     <col collapsed="false" hidden="false" max="14" min="11" style="2" width="13.3886639676113"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="3" width="36.8502024291498"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="3" width="37.17004048583"/>
     <col collapsed="false" hidden="false" max="16" min="16" style="3" width="13.497975708502"/>
     <col collapsed="false" hidden="false" max="17" min="17" style="2" width="13.497975708502"/>
-    <col collapsed="false" hidden="false" max="18" min="18" style="2" width="20.995951417004"/>
+    <col collapsed="false" hidden="false" max="18" min="18" style="2" width="21.1012145748988"/>
     <col collapsed="false" hidden="false" max="27" min="19" style="2" width="13.497975708502"/>
     <col collapsed="false" hidden="false" max="1025" min="28" style="1" width="9.10526315789474"/>
   </cols>
@@ -5270,19 +5279,19 @@
         <v>182</v>
       </c>
       <c r="F2" s="10" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="G2" s="10" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="H2" s="10" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="I2" s="10" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="J2" s="10" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="K2" s="10" t="s">
         <v>42</v>
@@ -5293,14 +5302,14 @@
       <c r="M2" s="10"/>
       <c r="N2" s="10"/>
       <c r="O2" s="10" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="P2" s="10" t="s">
-        <v>167</v>
+        <v>93</v>
       </c>
       <c r="Q2" s="10"/>
       <c r="R2" s="10" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="S2" s="10" t="s">
         <v>35</v>
@@ -5327,7 +5336,7 @@
         <v>182</v>
       </c>
       <c r="F3" s="10" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="G3" s="10" t="s">
         <v>168</v>
@@ -5336,10 +5345,10 @@
         <v>169</v>
       </c>
       <c r="I3" s="10" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="J3" s="10" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="K3" s="10" t="s">
         <v>42</v>
@@ -5353,7 +5362,7 @@
         <v>170</v>
       </c>
       <c r="P3" s="10" t="s">
-        <v>167</v>
+        <v>93</v>
       </c>
       <c r="Q3" s="10"/>
       <c r="R3" s="10" t="s">
@@ -5384,19 +5393,19 @@
         <v>182</v>
       </c>
       <c r="F4" s="10" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="G4" s="10" t="s">
         <v>183</v>
       </c>
       <c r="H4" s="10" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="I4" s="10" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="J4" s="10" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="K4" s="10" t="s">
         <v>80</v>
@@ -5435,19 +5444,19 @@
         <v>182</v>
       </c>
       <c r="F5" s="10" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="G5" s="10" t="s">
         <v>184</v>
       </c>
       <c r="H5" s="10" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="I5" s="10" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="J5" s="10" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="K5" s="10" t="s">
         <v>80</v>
@@ -5486,19 +5495,19 @@
         <v>182</v>
       </c>
       <c r="F6" s="10" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="G6" s="10" t="s">
         <v>185</v>
       </c>
       <c r="H6" s="10" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="I6" s="10" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="J6" s="10" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="K6" s="10" t="s">
         <v>80</v>
@@ -5566,7 +5575,9 @@
       <c r="O7" s="10" t="s">
         <v>35</v>
       </c>
-      <c r="P7" s="10"/>
+      <c r="P7" s="10" t="s">
+        <v>93</v>
+      </c>
       <c r="Q7" s="10" t="s">
         <v>36</v>
       </c>
@@ -5599,7 +5610,7 @@
         <v>28</v>
       </c>
       <c r="G8" s="10" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="H8" s="10" t="s">
         <v>186</v>
@@ -5656,10 +5667,10 @@
         <v>28</v>
       </c>
       <c r="G9" s="10" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="H9" s="10" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="I9" s="10" t="s">
         <v>91</v>
@@ -5671,7 +5682,7 @@
         <v>33</v>
       </c>
       <c r="L9" s="10" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="M9" s="10" t="n">
         <v>0</v>
@@ -5680,7 +5691,9 @@
       <c r="O9" s="10" t="s">
         <v>39</v>
       </c>
-      <c r="P9" s="10"/>
+      <c r="P9" s="10" t="s">
+        <v>93</v>
+      </c>
       <c r="Q9" s="10" t="s">
         <v>36</v>
       </c>
@@ -5795,7 +5808,7 @@
         <v>45</v>
       </c>
       <c r="P11" s="10" t="s">
-        <v>167</v>
+        <v>93</v>
       </c>
       <c r="Q11" s="10"/>
       <c r="R11" s="10"/>
@@ -5928,19 +5941,19 @@
         <v>182</v>
       </c>
       <c r="F14" s="10" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="G14" s="10" t="s">
         <v>196</v>
       </c>
       <c r="H14" s="10" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="I14" s="10" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="J14" s="10" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="K14" s="10" t="s">
         <v>80</v>
@@ -5981,7 +5994,7 @@
         <v>182</v>
       </c>
       <c r="F15" s="10" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="G15" s="10" t="s">
         <v>198</v>
@@ -6038,7 +6051,7 @@
         <v>182</v>
       </c>
       <c r="F16" s="10" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="G16" s="10" t="s">
         <v>200</v>
@@ -6095,7 +6108,7 @@
         <v>182</v>
       </c>
       <c r="F17" s="10" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="G17" s="10" t="s">
         <v>201</v>
@@ -6152,7 +6165,7 @@
         <v>182</v>
       </c>
       <c r="F18" s="10" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="G18" s="10" t="s">
         <v>202</v>
@@ -6209,7 +6222,7 @@
         <v>182</v>
       </c>
       <c r="F19" s="10" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="G19" s="10" t="s">
         <v>203</v>
@@ -6266,7 +6279,7 @@
         <v>182</v>
       </c>
       <c r="F20" s="10" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="G20" s="10" t="s">
         <v>204</v>
@@ -6323,7 +6336,7 @@
         <v>182</v>
       </c>
       <c r="F21" s="10" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="G21" s="10" t="s">
         <v>205</v>
@@ -6384,13 +6397,13 @@
         <v>206</v>
       </c>
       <c r="H22" s="10" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="I22" s="10" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="J22" s="10" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="K22" s="10" t="s">
         <v>80</v>
@@ -6432,16 +6445,16 @@
         <v>76</v>
       </c>
       <c r="G23" s="10" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="H23" s="10" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="I23" s="10" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="J23" s="10" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="K23" s="10" t="s">
         <v>80</v>
@@ -6488,10 +6501,10 @@
         <v>207</v>
       </c>
       <c r="H24" s="13" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="I24" s="10" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="J24" s="10"/>
       <c r="K24" s="10" t="s">
@@ -6503,7 +6516,7 @@
       <c r="M24" s="10"/>
       <c r="N24" s="10"/>
       <c r="O24" s="13" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="P24" s="10"/>
       <c r="Q24" s="10" t="s">
@@ -6518,7 +6531,7 @@
       <c r="V24" s="10"/>
       <c r="W24" s="10"/>
       <c r="X24" s="10" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="Y24" s="10"/>
       <c r="Z24" s="10"/>
@@ -6593,16 +6606,16 @@
         <v>76</v>
       </c>
       <c r="G26" s="10" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="H26" s="10" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="I26" s="10" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="J26" s="10" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="K26" s="10" t="s">
         <v>80</v>
@@ -6677,7 +6690,7 @@
     </row>
     <row r="28" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
-  <autoFilter ref="A1:AA3"/>
+  <autoFilter ref="A1:AA27"/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
   <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
@@ -6697,13 +6710,13 @@
   <dimension ref="A1:B19"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B2" activeCellId="1" sqref="B57:B60 B2"/>
+      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="51.5222672064777"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="19.8178137651822"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="51.9514170040486"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="19.9230769230769"/>
     <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="9.10526315789474"/>
   </cols>
   <sheetData>
@@ -6878,14 +6891,14 @@
   <dimension ref="1:58"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B30" activeCellId="1" sqref="B57:B60 B30"/>
+      <selection pane="topLeft" activeCell="B30" activeCellId="0" sqref="B30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
     <col collapsed="false" hidden="false" max="2" min="1" style="19" width="9"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="20" width="35.8866396761134"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="21" width="36.8502024291498"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="20" width="36.2064777327935"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="21" width="37.17004048583"/>
     <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
@@ -7742,13 +7755,13 @@
   <dimension ref="1:2"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A6" activeCellId="1" sqref="B57:B60 A6"/>
+      <selection pane="topLeft" activeCell="A6" activeCellId="0" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="20" width="35.8866396761134"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="21" width="36.8502024291498"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="20" width="36.2064777327935"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="21" width="37.17004048583"/>
     <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
@@ -7810,21 +7823,21 @@
   </sheetPr>
   <dimension ref="1:301"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B57" activeCellId="0" sqref="B57:B60"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B57" activeCellId="0" sqref="B57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="21" width="16.3886639676113"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="21" width="45.8461538461538"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="19" width="30.8502024291498"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="19" width="30.4210526315789"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="21" width="46.2753036437247"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="19" width="31.17004048583"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="19" width="30.6356275303644"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="19" width="16.3886639676113"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="35.1336032388664"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="35.3481781376518"/>
     <col collapsed="false" hidden="false" max="7" min="7" style="0" width="16.3886639676113"/>
     <col collapsed="false" hidden="false" max="9" min="8" style="0" width="10.7125506072875"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="26.3522267206478"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="26.5668016194332"/>
     <col collapsed="false" hidden="false" max="1025" min="11" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
@@ -17311,12 +17324,12 @@
   <dimension ref="A1:A2"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A3" activeCellId="1" sqref="B57:B60 A3"/>
+      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="19.3886639676113"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="19.4939271255061"/>
     <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="9.10526315789474"/>
   </cols>
   <sheetData>
@@ -17349,7 +17362,7 @@
   <dimension ref="A1:A2"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="1" sqref="B57:B60 A2"/>
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
@@ -17387,15 +17400,15 @@
   <dimension ref="A1:D1"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="B57:B60 A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="23.4574898785425"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="23.6720647773279"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="26.7813765182186"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="31.7085020242915"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="23.5668016194332"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="23.8866396761134"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="26.995951417004"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="31.9230769230769"/>
     <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>

</xml_diff>

<commit_message>
Merge branches 'master' and 'PROS-9205-marsru-assortment-update-api' of bitbucket.org:traxtechnology/kpi_factory into PROS-9205-marsru-assortment-update-api
# Conflicts:
#	Projects/MARSRU2_SAND/LocalCalculations.py
</commit_message>
<xml_diff>
--- a/Projects/MARSRU2_SAND/Data/2019/MARS KPIs.xlsx
+++ b/Projects/MARSRU2_SAND/Data/2019/MARS KPIs.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="992" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="KPIs_Grocery" sheetId="1" state="visible" r:id="rId2"/>
@@ -25,7 +25,7 @@
     <definedName function="false" hidden="true" localSheetId="5" name="_xlnm._FilterDatabase" vbProcedure="false">'4254'!$A$1:$J$259</definedName>
     <definedName function="false" hidden="true" localSheetId="1" name="_xlnm._FilterDatabase" vbProcedure="false">KPIs_Drogerie!$A$1:$AC$27</definedName>
     <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">KPIs_Grocery!$A$1:$AC$63</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">KPIs_Grocery!$A$1:$AC$56</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">KPIs_Grocery!$A$1:$AC$63</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0" vbProcedure="false">KPIs_Grocery!$A$1:$AC$56</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">KPIs_Grocery!$A$1:$AC$56</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0" vbProcedure="false">KPIs_Grocery!$A$1:$AC$56</definedName>
@@ -39,6 +39,7 @@
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">KPIs_Grocery!$A$1:$AC$56</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">KPIs_Grocery!$A$1:$AC$56</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">KPIs_Grocery!$A$1:$AC$56</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">KPIs_Grocery!$A$1:$AC$56</definedName>
     <definedName function="false" hidden="false" localSheetId="1" name="_FilterDatabase_0" vbProcedure="false">KPIs_Drogerie!$B$1:$AC$1</definedName>
     <definedName function="false" hidden="false" localSheetId="1" name="_FilterDatabase_0_0" vbProcedure="false">KPIs_Drogerie!$B$1:$AC$1</definedName>
     <definedName function="false" hidden="false" localSheetId="1" name="_FilterDatabase_0_0_0" vbProcedure="false">KPIs_Drogerie!$B$1:$AC$1</definedName>
@@ -57,17 +58,17 @@
     <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0" vbProcedure="false">KPIs_Drogerie!$A$1:$AC$27</definedName>
     <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">KPIs_Drogerie!$A$1:$AC$27</definedName>
     <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0_0" vbProcedure="false">KPIs_Drogerie!$A$1:$AC$27</definedName>
-    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0_0_0" vbProcedure="false">KPIs_Drogerie!$A$1:$AC$3</definedName>
-    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0_0_0_0" vbProcedure="false">KPIs_Drogerie!$A$1:$AC$27</definedName>
-    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0_0_0_0_0" vbProcedure="false">KPIs_Drogerie!$A$1:$AC$3</definedName>
-    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0" vbProcedure="false">KPIs_Drogerie!$A$1:$AC$27</definedName>
-    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0" vbProcedure="false">KPIs_Drogerie!$A$1:$AC$3</definedName>
-    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0" vbProcedure="false">KPIs_Drogerie!$A$1:$AC$27</definedName>
-    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">KPIs_Drogerie!$A$1:$AC$3</definedName>
-    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">KPIs_Drogerie!$A$1:$AC$27</definedName>
-    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">KPIs_Drogerie!$A$1:$AC$3</definedName>
-    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">KPIs_Drogerie!$A$1:$AC$27</definedName>
-    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">KPIs_Drogerie!$A$1:$AC$3</definedName>
+    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0_0_0" vbProcedure="false">KPIs_Drogerie!$A$1:$AC$27</definedName>
+    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0_0_0_0" vbProcedure="false">KPIs_Drogerie!$A$1:$AC$3</definedName>
+    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0_0_0_0_0" vbProcedure="false">KPIs_Drogerie!$A$1:$AC$27</definedName>
+    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0" vbProcedure="false">KPIs_Drogerie!$A$1:$AC$3</definedName>
+    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0" vbProcedure="false">KPIs_Drogerie!$A$1:$AC$27</definedName>
+    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0" vbProcedure="false">KPIs_Drogerie!$A$1:$AC$3</definedName>
+    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">KPIs_Drogerie!$A$1:$AC$27</definedName>
+    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">KPIs_Drogerie!$A$1:$AC$3</definedName>
+    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">KPIs_Drogerie!$A$1:$AC$27</definedName>
+    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">KPIs_Drogerie!$A$1:$AC$3</definedName>
+    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">KPIs_Drogerie!$A$1:$AC$27</definedName>
     <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">KPIs_Drogerie!$A$1:$AC$3</definedName>
     <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">KPIs_Drogerie!$A$1:$AC$3</definedName>
     <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">KPIs_Drogerie!$A$1:$AC$3</definedName>
@@ -92,6 +93,7 @@
     <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">KPIs_Drogerie!$A$1:$AC$3</definedName>
     <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">KPIs_Drogerie!$A$1:$AC$3</definedName>
     <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">KPIs_Drogerie!$A$1:$AC$3</definedName>
+    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">KPIs_Drogerie!$A$1:$AC$3</definedName>
     <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase" vbProcedure="false">'4317'!$A$1:$C$54</definedName>
     <definedName function="false" hidden="false" localSheetId="5" name="_xlnm._FilterDatabase" vbProcedure="false">'4254'!$A$1:$J$259</definedName>
     <definedName function="false" hidden="false" localSheetId="5" name="_xlnm._FilterDatabase_0" vbProcedure="false">'4254'!$A$1:$J$259</definedName>
@@ -119,10 +121,11 @@
     <definedName function="false" hidden="false" localSheetId="5" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'4254'!$A$1:$J$259</definedName>
     <definedName function="false" hidden="false" localSheetId="5" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'4254'!$A$1:$J$259</definedName>
     <definedName function="false" hidden="false" localSheetId="5" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'4254'!$A$1:$J$259</definedName>
-    <definedName function="false" hidden="false" localSheetId="5" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'4254'!$A$2:$J$260</definedName>
-    <definedName function="false" hidden="false" localSheetId="5" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'4254'!$A$1:$J$259</definedName>
-    <definedName function="false" hidden="false" localSheetId="5" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'4254'!$A$2:$J$260</definedName>
+    <definedName function="false" hidden="false" localSheetId="5" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'4254'!$A$1:$J$259</definedName>
+    <definedName function="false" hidden="false" localSheetId="5" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'4254'!$A$2:$J$260</definedName>
+    <definedName function="false" hidden="false" localSheetId="5" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'4254'!$A$1:$J$259</definedName>
     <definedName function="false" hidden="false" localSheetId="5" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'4254'!$A$2:$J$260</definedName>
+    <definedName function="false" hidden="false" localSheetId="5" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'4254'!$A$2:$J$260</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -1793,29 +1796,31 @@
   <dimension ref="A1:AC63"/>
   <sheetViews>
     <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="K56" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="1" topLeftCell="K2" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="K1" activeCellId="0" sqref="K1"/>
-      <selection pane="bottomLeft" activeCell="A56" activeCellId="0" sqref="A56"/>
-      <selection pane="bottomRight" activeCell="K23" activeCellId="0" sqref="K23"/>
+      <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="O22" activeCellId="0" sqref="O22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="1" width="13.3886639676113"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="2" width="13.3886639676113"/>
-    <col collapsed="false" hidden="false" max="4" min="3" style="2" width="23.2429149797571"/>
+    <col collapsed="false" hidden="false" max="4" min="3" style="2" width="23.3522267206478"/>
     <col collapsed="false" hidden="false" max="7" min="5" style="2" width="13.3886639676113"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="2" width="30.6356275303644"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="2" width="106.477732793522"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="2" width="74.6599190283401"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="2" width="31.4939271255061"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="2" width="30.8502024291498"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="2" width="107.441295546559"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="2" width="75.3036437246964"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="2" width="31.7085020242915"/>
     <col collapsed="false" hidden="false" max="12" min="12" style="2" width="16.3886639676113"/>
-    <col collapsed="false" hidden="false" max="16" min="13" style="2" width="13.3886639676113"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="3" width="38.2429149797571"/>
+    <col collapsed="false" hidden="false" max="14" min="13" style="2" width="13.3886639676113"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="2" width="19.9878542510121"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="2" width="13.3886639676113"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="3" width="38.5627530364372"/>
     <col collapsed="false" hidden="false" max="18" min="18" style="3" width="13.497975708502"/>
     <col collapsed="false" hidden="false" max="19" min="19" style="2" width="13.497975708502"/>
-    <col collapsed="false" hidden="false" max="20" min="20" style="2" width="21.7449392712551"/>
+    <col collapsed="false" hidden="false" max="20" min="20" style="2" width="21.9595141700405"/>
     <col collapsed="false" hidden="false" max="29" min="21" style="2" width="13.497975708502"/>
     <col collapsed="false" hidden="false" max="1025" min="30" style="1" width="9.10526315789474"/>
   </cols>
@@ -1950,7 +1955,9 @@
       <c r="N2" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="O2" s="10"/>
+      <c r="O2" s="10" t="n">
+        <v>1</v>
+      </c>
       <c r="P2" s="10" t="n">
         <v>2</v>
       </c>
@@ -2013,7 +2020,9 @@
       <c r="N3" s="10" t="s">
         <v>41</v>
       </c>
-      <c r="O3" s="10"/>
+      <c r="O3" s="10" t="n">
+        <v>1</v>
+      </c>
       <c r="P3" s="10" t="n">
         <v>2</v>
       </c>
@@ -3043,7 +3052,9 @@
       <c r="N19" s="10" t="n">
         <v>776682</v>
       </c>
-      <c r="O19" s="10"/>
+      <c r="O19" s="10" t="n">
+        <v>1</v>
+      </c>
       <c r="P19" s="10" t="n">
         <v>8</v>
       </c>
@@ -3100,7 +3111,9 @@
       <c r="N20" s="10" t="s">
         <v>84</v>
       </c>
-      <c r="O20" s="10"/>
+      <c r="O20" s="10" t="n">
+        <v>0</v>
+      </c>
       <c r="P20" s="10"/>
       <c r="Q20" s="13" t="s">
         <v>85</v>
@@ -3159,7 +3172,9 @@
       <c r="N21" s="10" t="s">
         <v>84</v>
       </c>
-      <c r="O21" s="10"/>
+      <c r="O21" s="10" t="n">
+        <v>0</v>
+      </c>
       <c r="P21" s="10"/>
       <c r="Q21" s="13" t="s">
         <v>88</v>
@@ -3218,7 +3233,9 @@
       <c r="N22" s="10" t="s">
         <v>84</v>
       </c>
-      <c r="O22" s="10"/>
+      <c r="O22" s="10" t="n">
+        <v>1</v>
+      </c>
       <c r="P22" s="10"/>
       <c r="Q22" s="13" t="s">
         <v>91</v>
@@ -4436,7 +4453,9 @@
       <c r="N42" s="10" t="s">
         <v>84</v>
       </c>
-      <c r="O42" s="10"/>
+      <c r="O42" s="10" t="n">
+        <v>0</v>
+      </c>
       <c r="P42" s="10"/>
       <c r="Q42" s="15" t="s">
         <v>140</v>
@@ -4495,7 +4514,9 @@
       <c r="N43" s="10" t="s">
         <v>84</v>
       </c>
-      <c r="O43" s="10"/>
+      <c r="O43" s="10" t="n">
+        <v>0</v>
+      </c>
       <c r="P43" s="10"/>
       <c r="Q43" s="13" t="s">
         <v>143</v>
@@ -4554,7 +4575,9 @@
       <c r="N44" s="10" t="s">
         <v>84</v>
       </c>
-      <c r="O44" s="10"/>
+      <c r="O44" s="10" t="n">
+        <v>1</v>
+      </c>
       <c r="P44" s="10"/>
       <c r="Q44" s="13" t="s">
         <v>147</v>
@@ -4617,7 +4640,9 @@
       <c r="N45" s="10" t="s">
         <v>84</v>
       </c>
-      <c r="O45" s="10"/>
+      <c r="O45" s="10" t="n">
+        <v>1</v>
+      </c>
       <c r="P45" s="10"/>
       <c r="Q45" s="13" t="s">
         <v>153</v>
@@ -4676,7 +4701,9 @@
       <c r="N46" s="10" t="s">
         <v>84</v>
       </c>
-      <c r="O46" s="10"/>
+      <c r="O46" s="10" t="n">
+        <v>1</v>
+      </c>
       <c r="P46" s="10"/>
       <c r="Q46" s="13" t="s">
         <v>91</v>
@@ -4735,7 +4762,9 @@
       <c r="N47" s="10" t="s">
         <v>84</v>
       </c>
-      <c r="O47" s="10"/>
+      <c r="O47" s="10" t="n">
+        <v>1</v>
+      </c>
       <c r="P47" s="10"/>
       <c r="Q47" s="10" t="s">
         <v>159</v>
@@ -4796,7 +4825,9 @@
       <c r="N48" s="10" t="n">
         <v>3</v>
       </c>
-      <c r="O48" s="10"/>
+      <c r="O48" s="10" t="n">
+        <v>1</v>
+      </c>
       <c r="P48" s="10"/>
       <c r="Q48" s="10" t="s">
         <v>166</v>
@@ -4855,7 +4886,9 @@
       <c r="N49" s="10" t="n">
         <v>3</v>
       </c>
-      <c r="O49" s="10"/>
+      <c r="O49" s="10" t="n">
+        <v>1</v>
+      </c>
       <c r="P49" s="10"/>
       <c r="Q49" s="10" t="s">
         <v>170</v>
@@ -4918,7 +4951,9 @@
       <c r="N50" s="10" t="n">
         <v>3</v>
       </c>
-      <c r="O50" s="10"/>
+      <c r="O50" s="10" t="n">
+        <v>1</v>
+      </c>
       <c r="P50" s="10"/>
       <c r="Q50" s="10" t="s">
         <v>173</v>
@@ -4981,7 +5016,9 @@
       <c r="N51" s="10" t="s">
         <v>84</v>
       </c>
-      <c r="O51" s="10"/>
+      <c r="O51" s="10" t="n">
+        <v>1</v>
+      </c>
       <c r="P51" s="10" t="n">
         <v>1</v>
       </c>
@@ -5044,7 +5081,9 @@
       <c r="N52" s="10" t="s">
         <v>84</v>
       </c>
-      <c r="O52" s="10"/>
+      <c r="O52" s="10" t="n">
+        <v>1</v>
+      </c>
       <c r="P52" s="10" t="n">
         <v>1</v>
       </c>
@@ -5734,8 +5773,8 @@
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="19" width="13.3886639676113"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="43.3846153846154"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="19" width="21.2105263157895"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="43.7044534412956"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="19" width="21.3157894736842"/>
     <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
@@ -5774,10 +5813,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="39.8502024291498"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="38.9919028340081"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="40.17004048583"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="39.3117408906883"/>
     <col collapsed="false" hidden="false" max="5" min="3" style="0" width="8.57085020242915"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="37.4898785425101"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="37.7044534412955"/>
     <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
@@ -5917,7 +5956,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="53.668016194332"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="54.0931174089069"/>
     <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
@@ -5975,7 +6014,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="true">
+  <sheetPr filterMode="false">
     <tabColor rgb="FFCCFF00"/>
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
@@ -5986,26 +6025,26 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="K1" activeCellId="0" sqref="K1"/>
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="L13" activeCellId="0" sqref="L13"/>
+      <selection pane="bottomRight" activeCell="O24" activeCellId="0" sqref="O24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="1" width="13.3886639676113"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="2" width="13.3886639676113"/>
-    <col collapsed="false" hidden="false" max="4" min="3" style="2" width="23.2429149797571"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="2" width="19.1740890688259"/>
+    <col collapsed="false" hidden="false" max="4" min="3" style="2" width="23.3522267206478"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="2" width="19.3886639676113"/>
     <col collapsed="false" hidden="false" max="7" min="6" style="2" width="13.3886639676113"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="2" width="30.6356275303644"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="2" width="106.477732793522"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="2" width="74.6599190283401"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="2" width="31.4939271255061"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="2" width="30.8502024291498"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="2" width="107.441295546559"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="2" width="75.3036437246964"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="2" width="31.7085020242915"/>
     <col collapsed="false" hidden="false" max="12" min="12" style="2" width="16.3886639676113"/>
     <col collapsed="false" hidden="false" max="16" min="13" style="2" width="13.3886639676113"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="3" width="38.2429149797571"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="3" width="38.5627530364372"/>
     <col collapsed="false" hidden="false" max="18" min="18" style="3" width="13.497975708502"/>
     <col collapsed="false" hidden="false" max="19" min="19" style="2" width="13.497975708502"/>
-    <col collapsed="false" hidden="false" max="20" min="20" style="2" width="21.7449392712551"/>
+    <col collapsed="false" hidden="false" max="20" min="20" style="2" width="21.9595141700405"/>
     <col collapsed="false" hidden="false" max="29" min="21" style="2" width="13.497975708502"/>
     <col collapsed="false" hidden="false" max="1025" min="30" style="1" width="9.10526315789474"/>
   </cols>
@@ -6099,7 +6138,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="29.95" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="29.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="10"/>
       <c r="B2" s="10" t="n">
         <v>2019</v>
@@ -6138,7 +6177,9 @@
       <c r="N2" s="10" t="n">
         <v>3</v>
       </c>
-      <c r="O2" s="10"/>
+      <c r="O2" s="10" t="n">
+        <v>1</v>
+      </c>
       <c r="P2" s="10"/>
       <c r="Q2" s="10" t="s">
         <v>170</v>
@@ -6162,7 +6203,7 @@
       <c r="AB2" s="10"/>
       <c r="AC2" s="10"/>
     </row>
-    <row r="3" customFormat="false" ht="29.95" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="29.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="10"/>
       <c r="B3" s="10" t="n">
         <v>2019</v>
@@ -6201,7 +6242,9 @@
       <c r="N3" s="10" t="n">
         <v>3</v>
       </c>
-      <c r="O3" s="10"/>
+      <c r="O3" s="10" t="n">
+        <v>1</v>
+      </c>
       <c r="P3" s="10"/>
       <c r="Q3" s="10" t="s">
         <v>173</v>
@@ -6225,7 +6268,7 @@
       <c r="AB3" s="10"/>
       <c r="AC3" s="10"/>
     </row>
-    <row r="4" customFormat="false" ht="29.95" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="29.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="10"/>
       <c r="B4" s="10" t="n">
         <v>2019</v>
@@ -6282,7 +6325,7 @@
       <c r="AB4" s="10"/>
       <c r="AC4" s="10"/>
     </row>
-    <row r="5" customFormat="false" ht="29.95" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="29.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="10"/>
       <c r="B5" s="10" t="n">
         <v>2019</v>
@@ -6339,7 +6382,7 @@
       <c r="AB5" s="10"/>
       <c r="AC5" s="10"/>
     </row>
-    <row r="6" customFormat="false" ht="29.95" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="6" customFormat="false" ht="29.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="10"/>
       <c r="B6" s="10" t="n">
         <v>2019</v>
@@ -6396,7 +6439,7 @@
       <c r="AB6" s="10"/>
       <c r="AC6" s="10"/>
     </row>
-    <row r="7" customFormat="false" ht="29.95" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="7" customFormat="false" ht="29.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="10" t="n">
         <v>2261</v>
       </c>
@@ -6461,7 +6504,7 @@
       <c r="AB7" s="10"/>
       <c r="AC7" s="10"/>
     </row>
-    <row r="8" customFormat="false" ht="29.95" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="8" customFormat="false" ht="29.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="10" t="n">
         <v>2262</v>
       </c>
@@ -6524,7 +6567,7 @@
       <c r="AB8" s="10"/>
       <c r="AC8" s="10"/>
     </row>
-    <row r="9" customFormat="false" ht="29.95" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="9" customFormat="false" ht="29.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="10" t="n">
         <v>2265</v>
       </c>
@@ -6589,7 +6632,7 @@
       <c r="AB9" s="10"/>
       <c r="AC9" s="10"/>
     </row>
-    <row r="10" customFormat="false" ht="29.95" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="10" customFormat="false" ht="29.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="10" t="n">
         <v>2266</v>
       </c>
@@ -6652,7 +6695,7 @@
       <c r="AB10" s="10"/>
       <c r="AC10" s="10"/>
     </row>
-    <row r="11" customFormat="false" ht="29.95" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="11" customFormat="false" ht="29.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A11" s="10"/>
       <c r="B11" s="10" t="n">
         <v>2019</v>
@@ -6833,7 +6876,7 @@
       <c r="AB13" s="10"/>
       <c r="AC13" s="10"/>
     </row>
-    <row r="14" customFormat="false" ht="29.95" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="14" customFormat="false" ht="29.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A14" s="10"/>
       <c r="B14" s="10" t="n">
         <v>2019</v>
@@ -7331,7 +7374,7 @@
       <c r="AB21" s="10"/>
       <c r="AC21" s="10"/>
     </row>
-    <row r="22" customFormat="false" ht="29.95" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="22" customFormat="false" ht="29.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A22" s="10"/>
       <c r="B22" s="10" t="n">
         <v>2019</v>
@@ -7388,7 +7431,7 @@
       <c r="AB22" s="10"/>
       <c r="AC22" s="10"/>
     </row>
-    <row r="23" customFormat="false" ht="29.95" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="23" customFormat="false" ht="29.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A23" s="10"/>
       <c r="B23" s="10" t="n">
         <v>2019</v>
@@ -7445,7 +7488,7 @@
       <c r="AB23" s="10"/>
       <c r="AC23" s="10"/>
     </row>
-    <row r="24" customFormat="false" ht="29.95" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="24" customFormat="false" ht="29.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A24" s="10" t="n">
         <v>2316</v>
       </c>
@@ -7484,7 +7527,9 @@
       <c r="N24" s="10" t="s">
         <v>84</v>
       </c>
-      <c r="O24" s="10"/>
+      <c r="O24" s="10" t="n">
+        <v>1</v>
+      </c>
       <c r="P24" s="10"/>
       <c r="Q24" s="13" t="s">
         <v>147</v>
@@ -7508,7 +7553,7 @@
       <c r="AB24" s="10"/>
       <c r="AC24" s="10"/>
     </row>
-    <row r="25" customFormat="false" ht="29.95" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="25" customFormat="false" ht="29.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A25" s="10" t="s">
         <v>229</v>
       </c>
@@ -7547,7 +7592,9 @@
       <c r="N25" s="10" t="s">
         <v>84</v>
       </c>
-      <c r="O25" s="10"/>
+      <c r="O25" s="10" t="n">
+        <v>1</v>
+      </c>
       <c r="P25" s="10"/>
       <c r="Q25" s="13" t="s">
         <v>91</v>
@@ -7567,7 +7614,7 @@
       <c r="AB25" s="10"/>
       <c r="AC25" s="10"/>
     </row>
-    <row r="26" customFormat="false" ht="29.95" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="26" customFormat="false" ht="29.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A26" s="10"/>
       <c r="B26" s="10" t="n">
         <v>2019</v>
@@ -7624,7 +7671,7 @@
       <c r="AB26" s="10"/>
       <c r="AC26" s="10"/>
     </row>
-    <row r="27" customFormat="false" ht="29.95" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="27" customFormat="false" ht="29.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A27" s="10"/>
       <c r="B27" s="10" t="n">
         <v>2019</v>
@@ -7661,7 +7708,9 @@
       <c r="N27" s="10" t="s">
         <v>84</v>
       </c>
-      <c r="O27" s="10"/>
+      <c r="O27" s="10" t="n">
+        <v>1</v>
+      </c>
       <c r="P27" s="10"/>
       <c r="Q27" s="10"/>
       <c r="R27" s="10"/>
@@ -7721,13 +7770,7 @@
     <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
-  <autoFilter ref="A1:AC27">
-    <filterColumn colId="11">
-      <customFilters and="true">
-        <customFilter operator="equal" val="SKUs"/>
-      </customFilters>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="A1:AC27"/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
   <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
@@ -7752,8 +7795,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="53.668016194332"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="20.3522267206478"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="54.0931174089069"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="20.4615384615385"/>
     <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="9.10526315789474"/>
   </cols>
   <sheetData>
@@ -7934,8 +7977,8 @@
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
     <col collapsed="false" hidden="false" max="2" min="1" style="19" width="9"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="20" width="37.4898785425101"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="21" width="38.2429149797571"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="20" width="37.7044534412955"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="21" width="38.5627530364372"/>
     <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
@@ -8797,8 +8840,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="20" width="37.4898785425101"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="21" width="38.2429149797571"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="20" width="37.7044534412955"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="21" width="38.5627530364372"/>
     <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
@@ -8867,14 +8910,14 @@
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="21" width="16.3886639676113"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="21" width="47.5627530364373"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="19" width="32.1376518218623"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="19" width="31.7085020242915"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="21" width="47.9878542510121"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="19" width="32.3481781376518"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="19" width="31.9230769230769"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="19" width="16.3886639676113"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="36.5263157894737"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="36.8502024291498"/>
     <col collapsed="false" hidden="false" max="7" min="7" style="0" width="16.3886639676113"/>
     <col collapsed="false" hidden="false" max="9" min="8" style="0" width="10.7125506072875"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="27.4210526315789"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="27.6356275303644"/>
     <col collapsed="false" hidden="false" max="1025" min="11" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
@@ -18366,7 +18409,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="19.9230769230769"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="20.0323886639676"/>
     <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="9.10526315789474"/>
   </cols>
   <sheetData>
@@ -18442,10 +18485,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="24.3157894736842"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="24.7449392712551"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="27.8502024291498"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="32.7773279352227"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="24.5303643724696"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="24.9595141700405"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="28.0647773279352"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="32.9919028340081"/>
     <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>

</xml_diff>